<commit_message>
Core always selected branch (needs testing)
</commit_message>
<xml_diff>
--- a/all_sources_in.xlsx
+++ b/all_sources_in.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/bq21582_bristol_ac_uk/Documents/Programs/web app/web-app/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_684983EFF8834D2A152C4C40952E2BBD78782E85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CE96E23-577D-4821-8786-9333150ED013}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="86280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="211">
   <si>
     <t>source</t>
   </si>
@@ -100,9 +106,6 @@
     <t>BIB</t>
   </si>
   <si>
-    <t>CORE</t>
-  </si>
-  <si>
     <t>ELSA</t>
   </si>
   <si>
@@ -173,9 +176,6 @@
   </si>
   <si>
     <t>Born in Bradford (BiB)</t>
-  </si>
-  <si>
-    <t>todo</t>
   </si>
   <si>
     <t>English Longitudinal Study of Ageing (ELSA)</t>
@@ -667,8 +667,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -731,13 +731,25 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -775,7 +787,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -809,6 +821,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -843,9 +856,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1018,14 +1032,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="32.765625" customWidth="1"/>
+    <col min="2" max="2" width="23.921875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1075,39 +1095,39 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I2" t="s">
         <v>163</v>
       </c>
-      <c r="I2" t="s">
-        <v>165</v>
-      </c>
       <c r="J2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L2">
         <v>1993</v>
@@ -1116,48 +1136,48 @@
         <v>30000</v>
       </c>
       <c r="N2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="O2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L3">
         <v>2013</v>
@@ -1166,48 +1186,48 @@
         <v>11000</v>
       </c>
       <c r="N3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="O3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="L4">
         <v>2005</v>
@@ -1216,48 +1236,48 @@
         <v>12435</v>
       </c>
       <c r="N4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="O4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H5" t="s">
+        <v>162</v>
+      </c>
+      <c r="I5" t="s">
         <v>164</v>
       </c>
-      <c r="I5" t="s">
-        <v>166</v>
-      </c>
       <c r="J5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L5">
         <v>2018</v>
@@ -1266,48 +1286,48 @@
         <v>40000</v>
       </c>
       <c r="N5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="O5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H6" t="s">
+        <v>162</v>
+      </c>
+      <c r="I6" t="s">
         <v>164</v>
       </c>
-      <c r="I6" t="s">
-        <v>166</v>
-      </c>
       <c r="J6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L6">
         <v>2020</v>
@@ -1316,45 +1336,45 @@
         <v>150000</v>
       </c>
       <c r="N6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="O6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K7">
         <v>1946</v>
@@ -1366,48 +1386,48 @@
         <v>5362</v>
       </c>
       <c r="N7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L8">
         <v>2020</v>
@@ -1416,48 +1436,48 @@
         <v>20000</v>
       </c>
       <c r="N8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="O8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P8" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H9" t="s">
+        <v>162</v>
+      </c>
+      <c r="I9" t="s">
         <v>164</v>
       </c>
-      <c r="I9" t="s">
-        <v>166</v>
-      </c>
       <c r="J9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L9">
         <v>2021</v>
@@ -1466,48 +1486,48 @@
         <v>18000</v>
       </c>
       <c r="N9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="O9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P9" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L10">
         <v>2004</v>
@@ -1516,95 +1536,95 @@
         <v>53000</v>
       </c>
       <c r="N10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="O10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P10" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H11" t="s">
+        <v>161</v>
+      </c>
+      <c r="I11" t="s">
         <v>163</v>
       </c>
-      <c r="I11" t="s">
-        <v>165</v>
-      </c>
       <c r="J11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K11" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="L11">
         <v>1990</v>
       </c>
       <c r="M11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="N11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P11" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K12">
         <v>1970</v>
@@ -1613,716 +1633,666 @@
         <v>1970</v>
       </c>
       <c r="M12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="N12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L13">
         <v>2007</v>
       </c>
       <c r="M13" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P13" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
       <c r="F14" t="s">
-        <v>53</v>
+        <v>140</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>154</v>
       </c>
       <c r="H14" t="s">
-        <v>53</v>
+        <v>162</v>
       </c>
       <c r="I14" t="s">
-        <v>53</v>
+        <v>163</v>
       </c>
       <c r="J14" t="s">
-        <v>53</v>
+        <v>172</v>
       </c>
       <c r="K14" t="s">
-        <v>53</v>
-      </c>
-      <c r="L14" t="s">
-        <v>53</v>
+        <v>177</v>
+      </c>
+      <c r="L14">
+        <v>2002</v>
       </c>
       <c r="M14" t="s">
-        <v>53</v>
+        <v>189</v>
       </c>
       <c r="N14" t="s">
-        <v>53</v>
+        <v>201</v>
       </c>
       <c r="O14" t="s">
-        <v>53</v>
+        <v>208</v>
       </c>
       <c r="P14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F15" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G15" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="H15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K15" t="s">
-        <v>179</v>
-      </c>
-      <c r="L15">
-        <v>2002</v>
+        <v>177</v>
+      </c>
+      <c r="L15" t="s">
+        <v>184</v>
       </c>
       <c r="M15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P15" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F16" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="G16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I16" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="J16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K16" t="s">
-        <v>179</v>
-      </c>
-      <c r="L16" t="s">
-        <v>186</v>
-      </c>
-      <c r="M16" t="s">
-        <v>192</v>
+        <v>181</v>
+      </c>
+      <c r="L16">
+        <v>2004</v>
+      </c>
+      <c r="M16">
+        <v>15770</v>
       </c>
       <c r="N16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P16" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H17" t="s">
+        <v>162</v>
+      </c>
+      <c r="I17" t="s">
         <v>164</v>
       </c>
-      <c r="I17" t="s">
-        <v>165</v>
-      </c>
       <c r="J17" t="s">
-        <v>174</v>
-      </c>
-      <c r="K17" t="s">
-        <v>183</v>
+        <v>172</v>
+      </c>
+      <c r="K17">
+        <v>2000</v>
       </c>
       <c r="L17">
-        <v>2004</v>
-      </c>
-      <c r="M17">
-        <v>15770</v>
+        <v>2000</v>
+      </c>
+      <c r="M17" t="s">
+        <v>191</v>
       </c>
       <c r="N17" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="O17" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P17" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K18">
-        <v>2000</v>
+        <v>1958</v>
       </c>
       <c r="L18">
-        <v>2000</v>
+        <v>1958</v>
       </c>
       <c r="M18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O18" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P18" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F19" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="G19" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I19" t="s">
         <v>167</v>
       </c>
       <c r="J19" t="s">
-        <v>174</v>
-      </c>
-      <c r="K19">
-        <v>1958</v>
+        <v>172</v>
+      </c>
+      <c r="K19" t="s">
+        <v>177</v>
       </c>
       <c r="L19">
-        <v>1958</v>
-      </c>
-      <c r="M19" t="s">
-        <v>194</v>
+        <v>2014</v>
+      </c>
+      <c r="M19">
+        <v>8504</v>
       </c>
       <c r="N19" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="O19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P19" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F20" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G20" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="H20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I20" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="J20" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K20" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="L20">
-        <v>2014</v>
+        <v>1988</v>
       </c>
       <c r="M20">
-        <v>8504</v>
+        <v>4858</v>
       </c>
       <c r="N20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O20" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P20" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F21" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G21" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="H21" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I21" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="J21" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L21">
-        <v>1988</v>
-      </c>
-      <c r="M21">
-        <v>4858</v>
+        <v>1994</v>
+      </c>
+      <c r="M21" t="s">
+        <v>193</v>
       </c>
       <c r="N21" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="O21" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P21" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F22" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="G22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I22" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J22" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K22" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="L22">
-        <v>1994</v>
+        <v>2009</v>
       </c>
       <c r="M22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N22" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="O22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P22" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F23" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="G23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H23" t="s">
+        <v>161</v>
+      </c>
+      <c r="I23" t="s">
         <v>164</v>
       </c>
-      <c r="I23" t="s">
-        <v>166</v>
-      </c>
       <c r="J23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L23">
-        <v>2009</v>
+        <v>1992</v>
       </c>
       <c r="M23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N23" t="s">
-        <v>179</v>
+        <v>206</v>
       </c>
       <c r="O23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P23" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F24" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="G24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H24" t="s">
+        <v>161</v>
+      </c>
+      <c r="I24" t="s">
         <v>163</v>
       </c>
-      <c r="I24" t="s">
-        <v>166</v>
-      </c>
       <c r="J24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="L24">
-        <v>1992</v>
+        <v>1998</v>
       </c>
       <c r="M24" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="N24" t="s">
+        <v>207</v>
+      </c>
+      <c r="O24" t="s">
         <v>208</v>
       </c>
-      <c r="O24" t="s">
+      <c r="P24" t="s">
         <v>210</v>
       </c>
-      <c r="P24" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16">
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K25" t="s">
-        <v>179</v>
-      </c>
-      <c r="L25">
-        <v>1998</v>
+        <v>177</v>
+      </c>
+      <c r="L25" t="s">
+        <v>185</v>
       </c>
       <c r="M25" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="N25" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O25" t="s">
+        <v>208</v>
+      </c>
+      <c r="P25" t="s">
         <v>210</v>
-      </c>
-      <c r="P25" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" t="s">
-        <v>113</v>
-      </c>
-      <c r="E26" t="s">
-        <v>137</v>
-      </c>
-      <c r="F26" t="s">
-        <v>150</v>
-      </c>
-      <c r="G26" t="s">
-        <v>162</v>
-      </c>
-      <c r="H26" t="s">
-        <v>164</v>
-      </c>
-      <c r="I26" t="s">
-        <v>166</v>
-      </c>
-      <c r="J26" t="s">
-        <v>174</v>
-      </c>
-      <c r="K26" t="s">
-        <v>179</v>
-      </c>
-      <c r="L26" t="s">
-        <v>187</v>
-      </c>
-      <c r="M26" t="s">
-        <v>187</v>
-      </c>
-      <c r="N26" t="s">
-        <v>209</v>
-      </c>
-      <c r="O26" t="s">
-        <v>210</v>
-      </c>
-      <c r="P26" t="s">
-        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>